<commit_message>
Updating open source files.
</commit_message>
<xml_diff>
--- a/CAD/Change Log.xlsx
+++ b/CAD/Change Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\TAVU\SOLDERED products\Soldered products\Aktuatori-black\Display OLED I2C White 0.96\CAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tavu\SOLDERED products\Soldered products\Aktuatori-black\Display OLED I2C White 0.96\CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>CHANGE LOG</t>
   </si>
@@ -96,6 +96,24 @@
   </si>
   <si>
     <t>v1.2.2.</t>
+  </si>
+  <si>
+    <t>Luka R.</t>
+  </si>
+  <si>
+    <t>25.11.2022.</t>
+  </si>
+  <si>
+    <t>Updated OLED footprint</t>
+  </si>
+  <si>
+    <t>New logos</t>
+  </si>
+  <si>
+    <t>v1.3.0.</t>
+  </si>
+  <si>
+    <t>25.12.2022.</t>
   </si>
 </sst>
 </file>
@@ -621,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -634,8 +652,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -666,6 +682,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -688,27 +726,8 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -995,7 +1014,7 @@
   <dimension ref="A1:Z1009"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:G21"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1010,14 +1029,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="75.75" customHeight="1">
-      <c r="A1" s="53"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="52"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1066,16 +1085,16 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="27" customHeight="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="61"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="60"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1124,18 +1143,18 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="15">
-      <c r="A5" s="14"/>
-      <c r="B5" s="56" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="15" t="s">
-        <v>21</v>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="13" t="s">
+        <v>26</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1156,18 +1175,18 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="14"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="56" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="19" t="s">
+      <c r="D6" s="56"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="17"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1188,18 +1207,18 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="15">
-      <c r="A7" s="14"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="56" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="19" t="s">
-        <v>20</v>
+      <c r="D7" s="56"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="17" t="s">
+        <v>27</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="17"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="15"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1220,18 +1239,18 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="15">
-      <c r="A8" s="14"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="56" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="19" t="s">
-        <v>11</v>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="17" t="s">
+        <v>22</v>
       </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="17"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1252,14 +1271,14 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="15">
-      <c r="A9" s="14"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="17"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1280,14 +1299,14 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" thickBot="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="17"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="15"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1308,26 +1327,26 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="16.5" thickTop="1">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="21" t="s">
+      <c r="D11" s="40"/>
+      <c r="E11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="34"/>
+      <c r="H11" s="42"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1348,16 +1367,16 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="37"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="45"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1378,16 +1397,16 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" thickBot="1">
-      <c r="A13" s="23"/>
-      <c r="B13" s="50" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="24"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="22"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1408,14 +1427,14 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="30"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1436,26 +1455,26 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="16.5" thickTop="1">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="21" t="s">
+      <c r="D15" s="40"/>
+      <c r="E15" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="34"/>
+      <c r="H15" s="42"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1476,16 +1495,16 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1506,16 +1525,16 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="25"/>
-      <c r="B17" s="44" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="26"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="24"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1536,16 +1555,16 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="25"/>
-      <c r="B18" s="44" t="s">
+      <c r="A18" s="23"/>
+      <c r="B18" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="26"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="24"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1566,16 +1585,16 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="25"/>
-      <c r="B19" s="44" t="s">
+      <c r="A19" s="23"/>
+      <c r="B19" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="26"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="24"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1596,14 +1615,14 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26">
-      <c r="A20" s="25"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="26"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="24"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1624,14 +1643,14 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26">
-      <c r="A21" s="25"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="26"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="24"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1652,14 +1671,14 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26">
-      <c r="A22" s="25"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="26"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="24"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1680,14 +1699,14 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26">
-      <c r="A23" s="25"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="26"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="24"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1708,14 +1727,14 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26">
-      <c r="A24" s="25"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="26"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="24"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1736,14 +1755,14 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26">
-      <c r="A25" s="25"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="26"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="24"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1764,14 +1783,14 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" thickBot="1">
-      <c r="A26" s="23"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="24"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="22"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1792,14 +1811,14 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1820,26 +1839,26 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="16.5" thickTop="1">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="21" t="s">
+      <c r="D28" s="40"/>
+      <c r="E28" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G28" s="33" t="s">
+      <c r="G28" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="H28" s="34"/>
+      <c r="H28" s="42"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -1860,16 +1879,16 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="45"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -1890,16 +1909,16 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="25"/>
-      <c r="B30" s="44" t="s">
+      <c r="A30" s="23"/>
+      <c r="B30" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="26"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="24"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -1920,14 +1939,14 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26">
-      <c r="A31" s="25"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="26"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="24"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -1948,14 +1967,14 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26">
-      <c r="A32" s="25"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="26"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="24"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1976,14 +1995,14 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26">
-      <c r="A33" s="25"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="26"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="24"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -2004,14 +2023,14 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26">
-      <c r="A34" s="25"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="26"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="24"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -2032,14 +2051,14 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26">
-      <c r="A35" s="25"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="26"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="24"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2060,14 +2079,14 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26">
-      <c r="A36" s="25"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="26"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="24"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -2088,14 +2107,14 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26">
-      <c r="A37" s="25"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="26"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="24"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -2116,14 +2135,14 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26">
-      <c r="A38" s="25"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="26"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="24"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -2144,14 +2163,14 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" thickBot="1">
-      <c r="A39" s="23"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="24"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="22"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -2172,14 +2191,14 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A40" s="28"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="30"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="38"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -2199,15 +2218,27 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" spans="1:26" ht="13.5" thickTop="1">
-      <c r="A41" s="2"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="3"/>
+    <row r="41" spans="1:26" ht="16.5" thickTop="1">
+      <c r="A41" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="40"/>
+      <c r="E41" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" s="42"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -2227,15 +2258,17 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" spans="1:26" ht="12.75">
-      <c r="A42" s="2"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="3"/>
+    <row r="42" spans="1:26">
+      <c r="A42" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="45"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -2255,15 +2288,17 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" spans="1:26" ht="12.75">
-      <c r="A43" s="2"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="3"/>
+    <row r="43" spans="1:26">
+      <c r="A43" s="23"/>
+      <c r="B43" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="24"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
@@ -2283,15 +2318,17 @@
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
     </row>
-    <row r="44" spans="1:26" ht="12.75">
-      <c r="A44" s="2"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="3"/>
+    <row r="44" spans="1:26">
+      <c r="A44" s="23"/>
+      <c r="B44" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="24"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
@@ -2311,15 +2348,15 @@
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
     </row>
-    <row r="45" spans="1:26" ht="12.75">
-      <c r="A45" s="2"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="3"/>
+    <row r="45" spans="1:26">
+      <c r="A45" s="23"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="24"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
@@ -2339,15 +2376,15 @@
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
     </row>
-    <row r="46" spans="1:26" ht="12.75">
-      <c r="A46" s="12"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="11"/>
+    <row r="46" spans="1:26">
+      <c r="A46" s="23"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="24"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
@@ -2367,15 +2404,15 @@
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" spans="1:26" ht="12.75">
-      <c r="A47" s="12"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="11"/>
+    <row r="47" spans="1:26">
+      <c r="A47" s="23"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="24"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -2395,15 +2432,15 @@
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
     </row>
-    <row r="48" spans="1:26" ht="12.75">
-      <c r="A48" s="12"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="11"/>
+    <row r="48" spans="1:26">
+      <c r="A48" s="23"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="24"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -2423,15 +2460,15 @@
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
     </row>
-    <row r="49" spans="1:26" ht="12.75">
-      <c r="A49" s="12"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="11"/>
+    <row r="49" spans="1:26">
+      <c r="A49" s="23"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="24"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
@@ -2451,15 +2488,15 @@
       <c r="Y49" s="1"/>
       <c r="Z49" s="1"/>
     </row>
-    <row r="50" spans="1:26" ht="12.75">
-      <c r="A50" s="12"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="11"/>
+    <row r="50" spans="1:26">
+      <c r="A50" s="23"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="24"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -2479,15 +2516,15 @@
       <c r="Y50" s="1"/>
       <c r="Z50" s="1"/>
     </row>
-    <row r="51" spans="1:26" ht="12.75">
-      <c r="A51" s="12"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="11"/>
+    <row r="51" spans="1:26">
+      <c r="A51" s="23"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="24"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -2507,15 +2544,15 @@
       <c r="Y51" s="1"/>
       <c r="Z51" s="1"/>
     </row>
-    <row r="52" spans="1:26" ht="12.75">
-      <c r="A52" s="2"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="3"/>
+    <row r="52" spans="1:26" thickBot="1">
+      <c r="A52" s="21"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="22"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -2535,7 +2572,7 @@
       <c r="Y52" s="1"/>
       <c r="Z52" s="1"/>
     </row>
-    <row r="53" spans="1:26" ht="12.75">
+    <row r="53" spans="1:26" ht="13.5" thickTop="1">
       <c r="A53" s="2"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -29332,31 +29369,20 @@
       <c r="Z1009" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A3:H3"/>
+  <mergeCells count="52">
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="A42:H42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:G44"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="C15:D15"/>
@@ -29372,6 +29398,30 @@
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B24:G24"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>